<commit_message>
added docs for tridev pcb
</commit_message>
<xml_diff>
--- a/pcb/tridev/rev_a/tridev_bom.xlsx
+++ b/pcb/tridev/rev_a/tridev_bom.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="146">
   <si>
     <t>Qty</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>CONSMA003.062-ND</t>
+  </si>
+  <si>
+    <t>y</t>
   </si>
   <si>
     <t>FRACTUS-2.4GHZ-FR05-S1-N-0-102</t>
@@ -576,10 +579,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -650,28 +653,34 @@
       <c r="G2" s="0" t="s">
         <v>14</v>
       </c>
+      <c r="K2" s="0" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -679,25 +688,28 @@
         <v>1</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+      <c r="K4" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -705,22 +717,25 @@
         <v>1</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
+      </c>
+      <c r="K5" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -728,22 +743,25 @@
         <v>2</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -751,22 +769,25 @@
         <v>2</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="K7" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -774,22 +795,25 @@
         <v>1</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
+      </c>
+      <c r="K8" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -797,22 +821,25 @@
         <v>1</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="K9" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -820,22 +847,25 @@
         <v>1</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -843,22 +873,25 @@
         <v>1</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
+      </c>
+      <c r="K11" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -866,22 +899,25 @@
         <v>11</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
+      </c>
+      <c r="K12" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -889,22 +925,25 @@
         <v>2</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
+      </c>
+      <c r="K13" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -912,22 +951,25 @@
         <v>3</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
+      </c>
+      <c r="K14" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -935,22 +977,25 @@
         <v>2</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
+      </c>
+      <c r="K15" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -958,22 +1003,25 @@
         <v>1</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
+      </c>
+      <c r="K16" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -981,22 +1029,25 @@
         <v>2</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
+      </c>
+      <c r="K17" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1004,22 +1055,25 @@
         <v>1</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
+      </c>
+      <c r="K18" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1027,28 +1081,31 @@
         <v>1</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
+      </c>
+      <c r="K19" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1056,19 +1113,22 @@
         <v>1</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
+      </c>
+      <c r="K20" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1076,16 +1136,19 @@
         <v>2</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
+      </c>
+      <c r="K21" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,19 +1156,22 @@
         <v>1</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
+      </c>
+      <c r="K22" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1113,19 +1179,22 @@
         <v>1</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="G23" s="2" t="s">
-        <v>99</v>
+        <v>100</v>
+      </c>
+      <c r="K23" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1133,19 +1202,22 @@
         <v>3</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>102</v>
+        <v>103</v>
+      </c>
+      <c r="K24" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1153,22 +1225,25 @@
         <v>4</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>108</v>
+        <v>109</v>
+      </c>
+      <c r="K25" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1176,22 +1251,25 @@
         <v>2</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>111</v>
+        <v>112</v>
+      </c>
+      <c r="K26" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1199,22 +1277,25 @@
         <v>1</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="G27" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
+      </c>
+      <c r="K27" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1222,19 +1303,22 @@
         <v>1</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>117</v>
+        <v>118</v>
+      </c>
+      <c r="K28" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1242,25 +1326,28 @@
         <v>1</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>123</v>
+        <v>124</v>
+      </c>
+      <c r="K29" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1268,22 +1355,25 @@
         <v>1</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
+      </c>
+      <c r="K30" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1291,28 +1381,31 @@
         <v>1</v>
       </c>
       <c r="B31" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="C31" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="D31" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>135</v>
+        <v>136</v>
+      </c>
+      <c r="K31" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1320,22 +1413,25 @@
         <v>1</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>140</v>
+        <v>141</v>
+      </c>
+      <c r="K32" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1343,19 +1439,22 @@
         <v>1</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>144</v>
+        <v>145</v>
+      </c>
+      <c r="K33" s="0" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update tridev with more jumpers
</commit_message>
<xml_diff>
--- a/pcb/tridev/rev_a/tridev_bom.xlsx
+++ b/pcb/tridev/rev_a/tridev_bom.xlsx
@@ -582,7 +582,7 @@
   <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+      <selection pane="topLeft" activeCell="A28" activeCellId="0" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1274,7 +1274,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>113</v>

</xml_diff>